<commit_message>
Cleaned EMaui model report to remove dummy 'mixed' scnearios.
</commit_message>
<xml_diff>
--- a/eastMaui/outputs/water_outputs.1.3.xlsx
+++ b/eastMaui/outputs/water_outputs.1.3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danwa\Documents\Programming\Trutta\HSHEP\EMaui\EMpackage\eastMaui\outputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{80354551-BE02-4C68-9AE6-9F815D598010}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41F54686-AC5D-470E-A94E-D9B25A97735D}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="9" r:id="rId1"/>
@@ -23,6 +23,9 @@
     <sheet name="springs" sheetId="7" r:id="rId8"/>
     <sheet name="sinks" sheetId="8" r:id="rId9"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId10"/>
+  </externalReferences>
   <calcPr calcId="179017"/>
 </workbook>
 </file>
@@ -7209,6 +7212,964 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Summary"/>
+      <sheetName val="WaterInDiversion"/>
+      <sheetName val="WaterInWatersheds"/>
+      <sheetName val="WaterInNodes"/>
+      <sheetName val="WaterByLease"/>
+      <sheetName val="taro"/>
+      <sheetName val="HabitatInWatersheds"/>
+      <sheetName val="AllSpeciesHab.nat.wsheds"/>
+      <sheetName val="AllSpHab.fullDiv.wsheds"/>
+      <sheetName val="AllSpHab.mixed.wsheds"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="3">
+          <cell r="C3" t="str">
+            <v>No Diversion</v>
+          </cell>
+          <cell r="D3" t="str">
+            <v>Sugar = Full Diversion</v>
+          </cell>
+          <cell r="E3" t="str">
+            <v>Mixed =  0.5</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="B4" t="str">
+            <v>Makapipi</v>
+          </cell>
+          <cell r="C4">
+            <v>2.6356807259999999</v>
+          </cell>
+          <cell r="D4">
+            <v>2.6356807259999999</v>
+          </cell>
+          <cell r="E4">
+            <v>2.6356807259999999</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="B5" t="str">
+            <v>Hanawi</v>
+          </cell>
+          <cell r="C5">
+            <v>13.487343156</v>
+          </cell>
+          <cell r="D5">
+            <v>11.574244836</v>
+          </cell>
+          <cell r="E5">
+            <v>12.1039016175</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="B6" t="str">
+            <v>Kapaula</v>
+          </cell>
+          <cell r="C6">
+            <v>3.0066666839999998</v>
+          </cell>
+          <cell r="D6">
+            <v>2.4818572799999998</v>
+          </cell>
+          <cell r="E6">
+            <v>2.6271170257500001</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="B7" t="str">
+            <v>Waiaaka</v>
+          </cell>
+          <cell r="C7">
+            <v>0.23590570499999999</v>
+          </cell>
+          <cell r="D7">
+            <v>0.21393092699999999</v>
+          </cell>
+          <cell r="E7">
+            <v>0.22491831600000001</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="B8" t="str">
+            <v>Paakea</v>
+          </cell>
+          <cell r="C8">
+            <v>1.314608778</v>
+          </cell>
+          <cell r="D8">
+            <v>0.72258240600000001</v>
+          </cell>
+          <cell r="E8">
+            <v>1.018595592</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="B9" t="str">
+            <v>Waiohue</v>
+          </cell>
+          <cell r="C9">
+            <v>1.6345356929999999</v>
+          </cell>
+          <cell r="D9">
+            <v>0.85507739100000002</v>
+          </cell>
+          <cell r="E9">
+            <v>1.2448065420000001</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="B10" t="str">
+            <v>Kopiliula</v>
+          </cell>
+          <cell r="C10">
+            <v>3.1630753980000001</v>
+          </cell>
+          <cell r="D10">
+            <v>1.704984246</v>
+          </cell>
+          <cell r="E10">
+            <v>2.3477465025000002</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="B11" t="str">
+            <v>East Wailua Iki</v>
+          </cell>
+          <cell r="C11">
+            <v>1.976437386</v>
+          </cell>
+          <cell r="D11">
+            <v>0.98110920599999996</v>
+          </cell>
+          <cell r="E11">
+            <v>1.478773296</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="B12" t="str">
+            <v>West Wailua Iki</v>
+          </cell>
+          <cell r="C12">
+            <v>2.1464187570000002</v>
+          </cell>
+          <cell r="D12">
+            <v>1.2435139079999999</v>
+          </cell>
+          <cell r="E12">
+            <v>1.6949663325</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="B13" t="str">
+            <v>Wailua Nui</v>
+          </cell>
+          <cell r="C13">
+            <v>5.4251848980000004</v>
+          </cell>
+          <cell r="D13">
+            <v>3.9748495500000001</v>
+          </cell>
+          <cell r="E13">
+            <v>4.6992093277500002</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="B14" t="str">
+            <v>Waiokamilo</v>
+          </cell>
+          <cell r="C14">
+            <v>2.7358598609999998</v>
+          </cell>
+          <cell r="D14">
+            <v>2.7358598609999998</v>
+          </cell>
+          <cell r="E14">
+            <v>2.7358598609999998</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="B15" t="str">
+            <v>Piinaau</v>
+          </cell>
+          <cell r="C15">
+            <v>11.647278656999999</v>
+          </cell>
+          <cell r="D15">
+            <v>9.6307696170000003</v>
+          </cell>
+          <cell r="E15">
+            <v>9.6307696170000003</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="B16" t="str">
+            <v>Nuaailua</v>
+          </cell>
+          <cell r="C16">
+            <v>3.9438263340000002</v>
+          </cell>
+          <cell r="D16">
+            <v>3.8249040060000001</v>
+          </cell>
+          <cell r="E16">
+            <v>3.8843651700000001</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="B17" t="str">
+            <v>Honomanu</v>
+          </cell>
+          <cell r="C17">
+            <v>5.2261192620000001</v>
+          </cell>
+          <cell r="D17">
+            <v>3.5263055520000002</v>
+          </cell>
+          <cell r="E17">
+            <v>4.2432326842499997</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="B18" t="str">
+            <v>Punalau</v>
+          </cell>
+          <cell r="C18">
+            <v>1.249330761</v>
+          </cell>
+          <cell r="D18">
+            <v>0.47698194599999999</v>
+          </cell>
+          <cell r="E18">
+            <v>0.59194558237499995</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="B19" t="str">
+            <v>Haipuaena</v>
+          </cell>
+          <cell r="C19">
+            <v>1.4761880279999999</v>
+          </cell>
+          <cell r="D19">
+            <v>0.69866867700000002</v>
+          </cell>
+          <cell r="E19">
+            <v>0.86372188087500001</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="B20" t="str">
+            <v>Puohokamoa</v>
+          </cell>
+          <cell r="C20">
+            <v>3.7247248709999998</v>
+          </cell>
+          <cell r="D20">
+            <v>1.010193471</v>
+          </cell>
+          <cell r="E20">
+            <v>1.4848325178749999</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="B21" t="str">
+            <v>Wahinepee</v>
+          </cell>
+          <cell r="C21">
+            <v>0.95590284299999995</v>
+          </cell>
+          <cell r="D21">
+            <v>0.87188163299999999</v>
+          </cell>
+          <cell r="E21">
+            <v>0.91389223799999997</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="B22" t="str">
+            <v>Waikamoi</v>
+          </cell>
+          <cell r="C22">
+            <v>1.946706804</v>
+          </cell>
+          <cell r="D22">
+            <v>0.29665950299999999</v>
+          </cell>
+          <cell r="E22">
+            <v>0.62046431999999996</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="B23" t="str">
+            <v>Kolea</v>
+          </cell>
+          <cell r="C23">
+            <v>1.2616107839999999</v>
+          </cell>
+          <cell r="D23">
+            <v>0.62240327100000004</v>
+          </cell>
+          <cell r="E23">
+            <v>0.69567946087499999</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="B24" t="str">
+            <v>Punaluu</v>
+          </cell>
+          <cell r="C24">
+            <v>0.365815422</v>
+          </cell>
+          <cell r="D24">
+            <v>0.144128691</v>
+          </cell>
+          <cell r="E24">
+            <v>0.25497205649999999</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="B25" t="str">
+            <v>Kaaiea</v>
+          </cell>
+          <cell r="C25">
+            <v>1.019241909</v>
+          </cell>
+          <cell r="D25">
+            <v>0.22039409700000001</v>
+          </cell>
+          <cell r="E25">
+            <v>0.32533981987499999</v>
+          </cell>
+        </row>
+        <row r="26">
+          <cell r="B26" t="str">
+            <v>Oopuola</v>
+          </cell>
+          <cell r="C26">
+            <v>1.829723427</v>
+          </cell>
+          <cell r="D26">
+            <v>1.019888226</v>
+          </cell>
+          <cell r="E26">
+            <v>1.1617548074999999</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="B27" t="str">
+            <v>Puehu</v>
+          </cell>
+          <cell r="C27">
+            <v>1.19568645</v>
+          </cell>
+          <cell r="D27">
+            <v>0.97141445100000001</v>
+          </cell>
+          <cell r="E27">
+            <v>1.0567282950000001</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="B28" t="str">
+            <v>Naiiliilihaele</v>
+          </cell>
+          <cell r="C28">
+            <v>6.2046431999999996</v>
+          </cell>
+          <cell r="D28">
+            <v>0.63209802599999998</v>
+          </cell>
+          <cell r="E28">
+            <v>1.026432185625</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="B29" t="str">
+            <v>Kailua</v>
+          </cell>
+          <cell r="C29">
+            <v>4.017506472</v>
+          </cell>
+          <cell r="D29">
+            <v>0.32445113399999997</v>
+          </cell>
+          <cell r="E29">
+            <v>0.57433344412499998</v>
+          </cell>
+        </row>
+        <row r="30">
+          <cell r="B30" t="str">
+            <v>Hanahana</v>
+          </cell>
+          <cell r="C30">
+            <v>1.2525623459999999</v>
+          </cell>
+          <cell r="D30">
+            <v>0.75425193899999998</v>
+          </cell>
+          <cell r="E30">
+            <v>0.98353289475000005</v>
+          </cell>
+        </row>
+        <row r="31">
+          <cell r="B31" t="str">
+            <v>Hoalua</v>
+          </cell>
+          <cell r="C31">
+            <v>2.046885939</v>
+          </cell>
+          <cell r="D31">
+            <v>0.287611065</v>
+          </cell>
+          <cell r="E31">
+            <v>0.63573355912499996</v>
+          </cell>
+        </row>
+        <row r="32">
+          <cell r="B32" t="str">
+            <v>Hanehoi</v>
+          </cell>
+          <cell r="C32">
+            <v>2.7462009329999999</v>
+          </cell>
+          <cell r="D32">
+            <v>1.1310547500000001</v>
+          </cell>
+          <cell r="E32">
+            <v>1.55584659825</v>
+          </cell>
+        </row>
+        <row r="33">
+          <cell r="B33" t="str">
+            <v>Waipionui</v>
+          </cell>
+          <cell r="C33">
+            <v>1.4076784259999999</v>
+          </cell>
+          <cell r="D33">
+            <v>1.4076784259999999</v>
+          </cell>
+          <cell r="E33">
+            <v>1.4076784259999999</v>
+          </cell>
+        </row>
+        <row r="34">
+          <cell r="B34" t="str">
+            <v>Waipio</v>
+          </cell>
+          <cell r="C34">
+            <v>1.1989180349999999</v>
+          </cell>
+          <cell r="D34">
+            <v>0.45888507000000001</v>
+          </cell>
+          <cell r="E34">
+            <v>0.69466959056249999</v>
+          </cell>
+        </row>
+        <row r="35">
+          <cell r="B35" t="str">
+            <v>Mokupapa</v>
+          </cell>
+          <cell r="C35">
+            <v>1.3811794289999999</v>
+          </cell>
+          <cell r="D35">
+            <v>0.77558039999999995</v>
+          </cell>
+          <cell r="E35">
+            <v>1.0551125025000001</v>
+          </cell>
+        </row>
+        <row r="36">
+          <cell r="B36" t="str">
+            <v>Honokala</v>
+          </cell>
+          <cell r="C36">
+            <v>1.4580911519999999</v>
+          </cell>
+          <cell r="D36">
+            <v>1.4580911519999999</v>
+          </cell>
+          <cell r="E36">
+            <v>1.4580911519999999</v>
+          </cell>
+        </row>
+        <row r="37">
+          <cell r="B37" t="str">
+            <v>Hoolawa</v>
+          </cell>
+          <cell r="C37">
+            <v>7.539934122</v>
+          </cell>
+          <cell r="D37">
+            <v>2.5807437809999998</v>
+          </cell>
+          <cell r="E37">
+            <v>3.3969209675625001</v>
+          </cell>
+        </row>
+        <row r="38">
+          <cell r="B38" t="str">
+            <v>Honopou</v>
+          </cell>
+          <cell r="C38">
+            <v>7.8585684029999996</v>
+          </cell>
+          <cell r="D38">
+            <v>4.2275594969999997</v>
+          </cell>
+          <cell r="E38">
+            <v>5.0002718653124996</v>
+          </cell>
+        </row>
+        <row r="39">
+          <cell r="B39" t="str">
+            <v>Halehaku</v>
+          </cell>
+          <cell r="C39">
+            <v>12.30587568</v>
+          </cell>
+          <cell r="D39">
+            <v>2.644082847</v>
+          </cell>
+          <cell r="E39">
+            <v>4.5077480152031297</v>
+          </cell>
+        </row>
+        <row r="40">
+          <cell r="B40" t="str">
+            <v>Peahi</v>
+          </cell>
+          <cell r="C40">
+            <v>0</v>
+          </cell>
+          <cell r="D40">
+            <v>0</v>
+          </cell>
+          <cell r="E40">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="41">
+          <cell r="B41" t="str">
+            <v>Kealii</v>
+          </cell>
+          <cell r="C41">
+            <v>1.368253089</v>
+          </cell>
+          <cell r="D41">
+            <v>1.1336400179999999</v>
+          </cell>
+          <cell r="E41">
+            <v>1.2509465534999999</v>
+          </cell>
+        </row>
+        <row r="42">
+          <cell r="B42" t="str">
+            <v>Uaoa</v>
+          </cell>
+          <cell r="C42">
+            <v>6.2098137360000001</v>
+          </cell>
+          <cell r="D42">
+            <v>1.952523657</v>
+          </cell>
+          <cell r="E42">
+            <v>3.11896426275</v>
+          </cell>
+        </row>
+        <row r="43">
+          <cell r="B43" t="str">
+            <v>Manawai</v>
+          </cell>
+          <cell r="C43">
+            <v>1.489760685</v>
+          </cell>
+          <cell r="D43">
+            <v>1.293926634</v>
+          </cell>
+          <cell r="E43">
+            <v>1.3918436595000001</v>
+          </cell>
+        </row>
+        <row r="44">
+          <cell r="B44" t="str">
+            <v>Holumalu</v>
+          </cell>
+          <cell r="C44">
+            <v>0</v>
+          </cell>
+          <cell r="D44">
+            <v>0</v>
+          </cell>
+          <cell r="E44">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="45">
+          <cell r="B45" t="str">
+            <v>Manawaiianu</v>
+          </cell>
+          <cell r="C45">
+            <v>4.2294984480000002</v>
+          </cell>
+          <cell r="D45">
+            <v>3.38023791</v>
+          </cell>
+          <cell r="E45">
+            <v>3.8048681790000001</v>
+          </cell>
+        </row>
+        <row r="46">
+          <cell r="B46" t="str">
+            <v>Opaepilau</v>
+          </cell>
+          <cell r="C46">
+            <v>5.9364216450000002</v>
+          </cell>
+          <cell r="D46">
+            <v>1.571196627</v>
+          </cell>
+          <cell r="E46">
+            <v>2.3425759665000001</v>
+          </cell>
+        </row>
+        <row r="47">
+          <cell r="B47" t="str">
+            <v>Konanui</v>
+          </cell>
+          <cell r="C47">
+            <v>1.719849537</v>
+          </cell>
+          <cell r="D47">
+            <v>1.4199584489999999</v>
+          </cell>
+          <cell r="E47">
+            <v>1.5699039930000001</v>
+          </cell>
+        </row>
+        <row r="48">
+          <cell r="B48" t="str">
+            <v>East Kuiaha</v>
+          </cell>
+          <cell r="C48">
+            <v>4.4305030350000001</v>
+          </cell>
+          <cell r="D48">
+            <v>2.574926928</v>
+          </cell>
+          <cell r="E48">
+            <v>3.3687657832500002</v>
+          </cell>
+        </row>
+        <row r="49">
+          <cell r="B49" t="str">
+            <v>Lilikoi</v>
+          </cell>
+          <cell r="C49">
+            <v>10.244770767</v>
+          </cell>
+          <cell r="D49">
+            <v>4.8868028370000003</v>
+          </cell>
+          <cell r="E49">
+            <v>6.7386626212499996</v>
+          </cell>
+        </row>
+        <row r="55">
+          <cell r="C55" t="str">
+            <v>No Diversion</v>
+          </cell>
+          <cell r="D55" t="str">
+            <v>Sugar = Full Diversion</v>
+          </cell>
+          <cell r="E55" t="str">
+            <v>Mixed = Diversion 0-1</v>
+          </cell>
+        </row>
+        <row r="57">
+          <cell r="B57" t="str">
+            <v>Center Ditch</v>
+          </cell>
+          <cell r="C57">
+            <v>0</v>
+          </cell>
+          <cell r="D57">
+            <v>8.7899112000000006</v>
+          </cell>
+          <cell r="E57">
+            <v>8.9870075888906307</v>
+          </cell>
+        </row>
+        <row r="58">
+          <cell r="B58" t="str">
+            <v>Haiku Ditch</v>
+          </cell>
+          <cell r="C58">
+            <v>0</v>
+          </cell>
+          <cell r="D58">
+            <v>16.976808639000001</v>
+          </cell>
+          <cell r="E58">
+            <v>10.08593836425</v>
+          </cell>
+        </row>
+        <row r="59">
+          <cell r="B59" t="str">
+            <v>Koolau Ditch</v>
+          </cell>
+          <cell r="C59">
+            <v>0</v>
+          </cell>
+          <cell r="D59">
+            <v>3.7673817930000002</v>
+          </cell>
+          <cell r="E59">
+            <v>2.6637147258749998</v>
+          </cell>
+        </row>
+        <row r="60">
+          <cell r="B60" t="str">
+            <v>Kauhikoa Ditch</v>
+          </cell>
+          <cell r="C60">
+            <v>0</v>
+          </cell>
+          <cell r="D60">
+            <v>13.530646395</v>
+          </cell>
+          <cell r="E60">
+            <v>10.1388959634375</v>
+          </cell>
+        </row>
+        <row r="61">
+          <cell r="B61" t="str">
+            <v>Lowrie Ditch</v>
+          </cell>
+          <cell r="C61">
+            <v>0</v>
+          </cell>
+          <cell r="D61">
+            <v>0.83310261299999999</v>
+          </cell>
+          <cell r="E61">
+            <v>1.007204254875</v>
+          </cell>
+        </row>
+        <row r="62">
+          <cell r="B62" t="str">
+            <v>Manuel Luis Ditch</v>
+          </cell>
+          <cell r="C62">
+            <v>0</v>
+          </cell>
+          <cell r="D62">
+            <v>2.4598825020000001</v>
+          </cell>
+          <cell r="E62">
+            <v>5.4589549612499999</v>
+          </cell>
+        </row>
+        <row r="63">
+          <cell r="B63" t="str">
+            <v>New Hamakua Ditch</v>
+          </cell>
+          <cell r="C63">
+            <v>0</v>
+          </cell>
+          <cell r="D63">
+            <v>5.4924018659999998</v>
+          </cell>
+          <cell r="E63">
+            <v>3.490515748125</v>
+          </cell>
+        </row>
+        <row r="64">
+          <cell r="B64" t="str">
+            <v>Spreckels Ditch</v>
+          </cell>
+          <cell r="C64">
+            <v>0</v>
+          </cell>
+          <cell r="D64">
+            <v>17.204312222999999</v>
+          </cell>
+          <cell r="E64">
+            <v>8.6021561114999994</v>
+          </cell>
+        </row>
+        <row r="65">
+          <cell r="B65" t="str">
+            <v>Wailoa Ditch</v>
+          </cell>
+          <cell r="C65">
+            <v>0</v>
+          </cell>
+          <cell r="D65">
+            <v>7.4087317710000002</v>
+          </cell>
+          <cell r="E65">
+            <v>4.8726040604062497</v>
+          </cell>
+        </row>
+        <row r="66">
+          <cell r="B66" t="str">
+            <v>Reservoirs</v>
+          </cell>
+          <cell r="C66">
+            <v>0</v>
+          </cell>
+          <cell r="D66">
+            <v>0</v>
+          </cell>
+          <cell r="E66">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="71">
+          <cell r="C71" t="str">
+            <v>No Diversion</v>
+          </cell>
+          <cell r="D71" t="str">
+            <v>Sugar = Full Diversion</v>
+          </cell>
+          <cell r="E71" t="str">
+            <v>Mixed = Diversion 0-1</v>
+          </cell>
+        </row>
+        <row r="73">
+          <cell r="A73" t="str">
+            <v>Honomanu</v>
+          </cell>
+          <cell r="C73">
+            <v>0</v>
+          </cell>
+          <cell r="D73">
+            <v>5.2119999999999997</v>
+          </cell>
+          <cell r="E73">
+            <v>3.4344999999999999</v>
+          </cell>
+        </row>
+        <row r="74">
+          <cell r="A74" t="str">
+            <v>Huelo</v>
+          </cell>
+          <cell r="C74">
+            <v>0</v>
+          </cell>
+          <cell r="D74">
+            <v>47.07</v>
+          </cell>
+          <cell r="E74">
+            <v>40.587687500000001</v>
+          </cell>
+        </row>
+        <row r="75">
+          <cell r="A75" t="str">
+            <v>Keanae</v>
+          </cell>
+          <cell r="C75">
+            <v>0</v>
+          </cell>
+          <cell r="D75">
+            <v>18.803000000000001</v>
+          </cell>
+          <cell r="E75">
+            <v>9.7632499999999993</v>
+          </cell>
+        </row>
+        <row r="76">
+          <cell r="A76" t="str">
+            <v>Nahiku</v>
+          </cell>
+          <cell r="C76">
+            <v>0</v>
+          </cell>
+          <cell r="D76">
+            <v>6.0679999999999996</v>
+          </cell>
+          <cell r="E76">
+            <v>3.87575</v>
+          </cell>
+        </row>
+        <row r="77">
+          <cell r="A77" t="str">
+            <v>Non Lease</v>
+          </cell>
+          <cell r="C77">
+            <v>0</v>
+          </cell>
+          <cell r="D77">
+            <v>45.710999999999999</v>
+          </cell>
+          <cell r="E77">
+            <v>32.982734375</v>
+          </cell>
+        </row>
+        <row r="82">
+          <cell r="C82" t="str">
+            <v>No Diversion</v>
+          </cell>
+          <cell r="D82" t="str">
+            <v>Sugar = Full Diversion</v>
+          </cell>
+          <cell r="E82" t="str">
+            <v>Mixed = Diversion 0-1</v>
+          </cell>
+        </row>
+        <row r="84">
+          <cell r="A84" t="str">
+            <v>Yes</v>
+          </cell>
+          <cell r="C84">
+            <v>0</v>
+          </cell>
+          <cell r="D84">
+            <v>12.649070007000001</v>
+          </cell>
+          <cell r="E84">
+            <v>7.8976301866874996</v>
+          </cell>
+        </row>
+        <row r="85">
+          <cell r="A85" t="str">
+            <v>No</v>
+          </cell>
+          <cell r="C85">
+            <v>0</v>
+          </cell>
+          <cell r="D85">
+            <v>66.760021881</v>
+          </cell>
+          <cell r="E85">
+            <v>50.687077467796897</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -7490,8 +8451,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D00F0CD-A8F4-4923-95EE-5C8A7EE13E28}">
   <dimension ref="A1:S85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="P55" sqref="P55"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>